<commit_message>
Add reviewed tweets REVIEWED_RandyFeenstra_20201027_20210101_20250924_autoPush.xlsx
</commit_message>
<xml_diff>
--- a/REVIEWED_RandyFeenstra_20201027_20210101_20250924_autoPush.xlsx
+++ b/REVIEWED_RandyFeenstra_20201027_20210101_20250924_autoPush.xlsx
@@ -542,7 +542,11 @@
       <c r="H3" t="b">
         <v>1</v>
       </c>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -573,7 +577,11 @@
       <c r="H4" t="b">
         <v>1</v>
       </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -602,7 +610,11 @@
       <c r="H5" t="b">
         <v>1</v>
       </c>
-      <c r="I5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -631,7 +643,11 @@
       <c r="H6" t="b">
         <v>1</v>
       </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -763,7 +779,11 @@
       <c r="H10" t="b">
         <v>1</v>
       </c>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -796,7 +816,11 @@
       <c r="H11" t="b">
         <v>1</v>
       </c>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -924,7 +948,11 @@
       <c r="H15" t="b">
         <v>1</v>
       </c>
-      <c r="I15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">

</xml_diff>